<commit_message>
Update schematics and readme for driver board.
</commit_message>
<xml_diff>
--- a/InstrumentBuild/PartsList20181210.xlsx
+++ b/InstrumentBuild/PartsList20181210.xlsx
@@ -1,23 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rustyn\Documents\diyOPT\AIBSopt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rustyn\Documents\diyOPT\AIBSopt\InstrumentBuild\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3160F6E-CD06-4555-A8A3-22C0224D54BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24765" windowHeight="10830"/>
+    <workbookView xWindow="705" yWindow="585" windowWidth="27300" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -209,9 +216,6 @@
     <t>B00NH11KIK</t>
   </si>
   <si>
-    <t>Must supply 18V @ 1 A</t>
-  </si>
-  <si>
     <t>0.9 degree; NEMA 17</t>
   </si>
   <si>
@@ -359,9 +363,6 @@
     <t>Motor driver Arduino shield</t>
   </si>
   <si>
-    <t>In-house design</t>
-  </si>
-  <si>
     <t>63-442</t>
   </si>
   <si>
@@ -384,12 +385,18 @@
   </si>
   <si>
     <t>SM1L03</t>
+  </si>
+  <si>
+    <t>Must supply 18V @ 1 A; 5.5 mm x 2.1 mm connector with optMotorDriver</t>
+  </si>
+  <si>
+    <t>In-house design; See ./AIBSopt/EAGLE/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -794,11 +801,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -816,7 +823,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -831,10 +838,10 @@
         <v>21</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
@@ -842,7 +849,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -919,7 +926,7 @@
         <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
@@ -935,13 +942,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E6" s="3">
         <v>3</v>
@@ -954,7 +961,7 @@
         <v>23.009999999999998</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -1013,7 +1020,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>8</v>
@@ -1044,7 +1051,7 @@
         <v>41</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1063,10 +1070,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
@@ -1110,7 +1117,7 @@
         <v>41</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" s="3">
         <v>1</v>
@@ -1148,13 +1155,13 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E16" s="3">
         <v>2</v>
@@ -1167,18 +1174,18 @@
         <v>25.18</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E17" s="3">
         <v>1</v>
@@ -1194,13 +1201,13 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E18" s="3">
         <v>0.2</v>
@@ -1216,13 +1223,13 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E19" s="3">
         <v>1</v>
@@ -1238,13 +1245,13 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B20" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E20" s="3">
         <v>1</v>
@@ -1268,7 +1275,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>12</v>
@@ -1293,13 +1300,13 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
@@ -1365,7 +1372,7 @@
         <v>41</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
@@ -1381,13 +1388,13 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E27" s="3">
         <v>0.2</v>
@@ -1403,13 +1410,13 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B28" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E28" s="3">
         <v>1</v>
@@ -1425,13 +1432,13 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B29" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E29" s="3">
         <v>1</v>
@@ -1499,7 +1506,7 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>15</v>
@@ -1530,7 +1537,7 @@
         <v>41</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
@@ -1543,18 +1550,18 @@
         <v>20.76</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B35" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="E35" s="3">
         <v>4</v>
@@ -1567,18 +1574,18 @@
         <v>30.8</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B36" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="E36" s="3">
         <v>4</v>
@@ -1600,7 +1607,7 @@
         <v>41</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E37" s="3">
         <v>1.6</v>
@@ -1613,7 +1620,7 @@
         <v>64.304000000000002</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1621,10 +1628,10 @@
         <v>18</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E38" s="3">
         <v>4</v>
@@ -1646,7 +1653,7 @@
         <v>41</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E39" s="3">
         <v>1</v>
@@ -1662,13 +1669,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -1692,16 +1699,16 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E42" s="3">
         <v>1</v>
@@ -1723,7 +1730,7 @@
         <v>41</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E43" s="3">
         <v>2</v>
@@ -1757,13 +1764,13 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B45" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D45" s="5" t="s">
         <v>78</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>79</v>
       </c>
       <c r="E45" s="3">
         <v>1</v>
@@ -1779,7 +1786,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B46" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>55</v>
@@ -1792,7 +1799,7 @@
       </c>
       <c r="F46" s="7"/>
       <c r="H46" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
@@ -1810,7 +1817,7 @@
       </c>
       <c r="F47" s="7"/>
       <c r="H47" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1833,13 +1840,13 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B49" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E49" s="3">
         <v>4</v>
@@ -1855,13 +1862,13 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B50" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E50" s="3">
         <v>0.8</v>
@@ -1885,7 +1892,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>26</v>
@@ -1894,7 +1901,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E52" s="3">
         <v>1</v>
@@ -1989,12 +1996,12 @@
       </c>
       <c r="F56" s="7"/>
       <c r="H56" s="3" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B57" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C57" s="5" t="s">
         <v>55</v>
@@ -2007,12 +2014,12 @@
       </c>
       <c r="F57" s="7"/>
       <c r="H57" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C58" s="5" t="s">
         <v>55</v>
@@ -2025,12 +2032,12 @@
       </c>
       <c r="F58" s="7"/>
       <c r="H58" s="3" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>28</v>
@@ -2046,12 +2053,12 @@
       </c>
       <c r="F60" s="7"/>
       <c r="H60" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="E62" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F62" s="8">
         <f>SUM(G2:G62)</f>
@@ -2060,8 +2067,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D15" r:id="rId1" display="https://www.thorlabs.com/thorproduct.cfm?partnumber=KPS101"/>
-    <hyperlink ref="D31" r:id="rId2" display="https://www.thorlabs.com/thorproduct.cfm?partnumber=KPS101"/>
+    <hyperlink ref="D15" r:id="rId1" display="https://www.thorlabs.com/thorproduct.cfm?partnumber=KPS101" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D31" r:id="rId2" display="https://www.thorlabs.com/thorproduct.cfm?partnumber=KPS101" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Added sheet for laserLaunch in ./InstrumentBuild/PartsList20181210.xlsx.  Sheet contains no data.
</commit_message>
<xml_diff>
--- a/InstrumentBuild/PartsList20181210.xlsx
+++ b/InstrumentBuild/PartsList20181210.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rustyn\Documents\diyOPT\AIBSopt\InstrumentBuild\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rusty Nicovich\Documents\CAD\OPT\aibsopt\InstrumentBuild\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3160F6E-CD06-4555-A8A3-22C0224D54BB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082063BE-D280-4800-8A57-121C3B6FB9F6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="585" windowWidth="27300" windowHeight="16650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2745" yWindow="735" windowWidth="26055" windowHeight="13605" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="DemoSystem" sheetId="1" r:id="rId1"/>
+    <sheet name="LaserLaunch" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="120">
   <si>
     <t>Component</t>
   </si>
@@ -804,7 +805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
@@ -2073,4 +2074,517 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{588022B8-37DA-44AF-8FCC-C245FFE34C48}">
+  <dimension ref="A1:H60"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15" style="8" customWidth="1"/>
+    <col min="8" max="8" width="45.140625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="3"/>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="7"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="7"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="7"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="7"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="7"/>
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="7"/>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="7"/>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="7"/>
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="7"/>
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="7"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="7"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="7"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="7"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="7"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="7"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="7"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="7"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="7"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="7"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="7"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="7"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="7"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="7"/>
+      <c r="H30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="7"/>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="7"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="7"/>
+      <c r="H33" s="3"/>
+    </row>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="7"/>
+      <c r="H34" s="3"/>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="7"/>
+      <c r="H35" s="3"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="7"/>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="7"/>
+      <c r="H37" s="3"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="7"/>
+      <c r="H38" s="3"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="3"/>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="7"/>
+      <c r="H39" s="3"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="7"/>
+      <c r="H40" s="3"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="7"/>
+      <c r="H41" s="3"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="7"/>
+      <c r="H42" s="3"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="7"/>
+      <c r="H43" s="3"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="3"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="7"/>
+      <c r="H44" s="3"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="3"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="7"/>
+      <c r="H45" s="3"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="3"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="7"/>
+      <c r="H46" s="3"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="3"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="7"/>
+      <c r="H47" s="3"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="3"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="7"/>
+      <c r="H48" s="3"/>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="7"/>
+      <c r="H49" s="3"/>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="7"/>
+      <c r="H50" s="3"/>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="7"/>
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B52" s="3"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="7"/>
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B53" s="3"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="3"/>
+      <c r="F53" s="7"/>
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="7"/>
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B55" s="3"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="7"/>
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B56" s="3"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="7"/>
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B57" s="3"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="7"/>
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B58" s="3"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="7"/>
+      <c r="H58" s="3"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="3"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="7"/>
+      <c r="H60" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>